<commit_message>
- Correction of fit_transform to transform as in class notebooks
</commit_message>
<xml_diff>
--- a/[ML]_Project_EDAOutputs_Group33/FeatureSelection/Lasso_Ridge_Coefficients_LogisticRegression.xlsx
+++ b/[ML]_Project_EDAOutputs_Group33/FeatureSelection/Lasso_Ridge_Coefficients_LogisticRegression.xlsx
@@ -457,10 +457,10 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.2828326948159203</v>
+        <v>0.2828091028781806</v>
       </c>
       <c r="C2" t="n">
-        <v>1.350240067153015</v>
+        <v>1.350255457431442</v>
       </c>
     </row>
     <row r="3">
@@ -470,10 +470,10 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.1414461048269697</v>
+        <v>0.1414338610909474</v>
       </c>
       <c r="C3" t="n">
-        <v>0.4984704101266608</v>
+        <v>0.4984775180341366</v>
       </c>
     </row>
     <row r="4">
@@ -483,10 +483,10 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.1413119565500388</v>
+        <v>0.1413210377033591</v>
       </c>
       <c r="C4" t="n">
-        <v>0.538719187006345</v>
+        <v>0.5387254751084597</v>
       </c>
     </row>
     <row r="5">
@@ -496,10 +496,10 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.1208203644679715</v>
+        <v>0.1208146547144282</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3269139564586553</v>
+        <v>0.3269234615657828</v>
       </c>
     </row>
     <row r="6">
@@ -509,10 +509,10 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.1025610361436726</v>
+        <v>0.1025752824159047</v>
       </c>
       <c r="C6" t="n">
-        <v>0.2181095824647866</v>
+        <v>0.2181173424761773</v>
       </c>
     </row>
     <row r="7">
@@ -522,10 +522,10 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.077569736915371</v>
+        <v>0.07755293685819994</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1321134826759434</v>
+        <v>0.1321136037614467</v>
       </c>
     </row>
     <row r="8">
@@ -535,10 +535,10 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.0516007230218438</v>
+        <v>0.05157801628554341</v>
       </c>
       <c r="C8" t="n">
-        <v>0.08296908406762714</v>
+        <v>0.0829643683544774</v>
       </c>
     </row>
     <row r="9">
@@ -548,10 +548,10 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.02469003602960787</v>
+        <v>0.02468426224702742</v>
       </c>
       <c r="C9" t="n">
-        <v>0.07304782532221903</v>
+        <v>0.07304461702684679</v>
       </c>
     </row>
     <row r="10">
@@ -561,10 +561,10 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.02416837142757404</v>
+        <v>0.02415204414363451</v>
       </c>
       <c r="C10" t="n">
-        <v>0.05645472842464471</v>
+        <v>0.05646152931300302</v>
       </c>
     </row>
     <row r="11">
@@ -574,10 +574,10 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.02302151915531528</v>
+        <v>0.02301148010812246</v>
       </c>
       <c r="C11" t="n">
-        <v>0.06897189817914931</v>
+        <v>0.0689758041438378</v>
       </c>
     </row>
     <row r="12">
@@ -587,10 +587,10 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.02129286469469621</v>
+        <v>0.02127505338232546</v>
       </c>
       <c r="C12" t="n">
-        <v>0.1476522095072208</v>
+        <v>0.1476674810891583</v>
       </c>
     </row>
     <row r="13">
@@ -600,10 +600,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>0.0211306455581645</v>
+        <v>0.02111811286677057</v>
       </c>
       <c r="C13" t="n">
-        <v>0.1076223104373248</v>
+        <v>0.1076348261615857</v>
       </c>
     </row>
     <row r="14">
@@ -613,10 +613,10 @@
         </is>
       </c>
       <c r="B14" t="n">
-        <v>0.01907274334526828</v>
+        <v>0.01907755748545021</v>
       </c>
       <c r="C14" t="n">
-        <v>0.05332708502388438</v>
+        <v>0.05332672429125075</v>
       </c>
     </row>
     <row r="15">
@@ -626,10 +626,10 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01765751251714762</v>
+        <v>0.01760807120149784</v>
       </c>
       <c r="C15" t="n">
-        <v>0.02622382314206724</v>
+        <v>0.02622394461014483</v>
       </c>
     </row>
     <row r="16">
@@ -639,10 +639,10 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>0.01235659631514574</v>
+        <v>0.01235963452270528</v>
       </c>
       <c r="C16" t="n">
-        <v>0.1471891782804789</v>
+        <v>0.1471725105760397</v>
       </c>
     </row>
     <row r="17">
@@ -652,10 +652,10 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>0.01204589790386476</v>
+        <v>0.01204075761044195</v>
       </c>
       <c r="C17" t="n">
-        <v>0.07019715783661432</v>
+        <v>0.07019464864212284</v>
       </c>
     </row>
     <row r="18">
@@ -665,10 +665,10 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01123338919405442</v>
+        <v>0.01122503701275782</v>
       </c>
       <c r="C18" t="n">
-        <v>0.01711672857931909</v>
+        <v>0.01711301379271353</v>
       </c>
     </row>
     <row r="19">
@@ -678,10 +678,10 @@
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.01058330557507288</v>
+        <v>0.01059433714471243</v>
       </c>
       <c r="C19" t="n">
-        <v>0.008402317855282709</v>
+        <v>0.008402331080290776</v>
       </c>
     </row>
     <row r="20">
@@ -691,10 +691,10 @@
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.008012867009806079</v>
+        <v>0.00800901066799071</v>
       </c>
       <c r="C20" t="n">
-        <v>0.02079806360113185</v>
+        <v>0.02079650453655959</v>
       </c>
     </row>
     <row r="21">
@@ -704,10 +704,10 @@
         </is>
       </c>
       <c r="B21" t="n">
-        <v>0.008002250620374544</v>
+        <v>0.0080081760197923</v>
       </c>
       <c r="C21" t="n">
-        <v>0.006492267339192637</v>
+        <v>0.006499775996258665</v>
       </c>
     </row>
     <row r="22">
@@ -717,10 +717,10 @@
         </is>
       </c>
       <c r="B22" t="n">
-        <v>0.007536680206718665</v>
+        <v>0.007533344571297384</v>
       </c>
       <c r="C22" t="n">
-        <v>0.09726326203554776</v>
+        <v>0.09726382449937171</v>
       </c>
     </row>
     <row r="23">
@@ -730,10 +730,10 @@
         </is>
       </c>
       <c r="B23" t="n">
-        <v>0.005831780443985647</v>
+        <v>0.005836917925507889</v>
       </c>
       <c r="C23" t="n">
-        <v>0.01132869516434925</v>
+        <v>0.0113298402098771</v>
       </c>
     </row>
     <row r="24">
@@ -743,10 +743,10 @@
         </is>
       </c>
       <c r="B24" t="n">
-        <v>0.005618174364234231</v>
+        <v>0.005616144775818515</v>
       </c>
       <c r="C24" t="n">
-        <v>0.01041345200874976</v>
+        <v>0.01041889623275816</v>
       </c>
     </row>
     <row r="25">
@@ -756,10 +756,10 @@
         </is>
       </c>
       <c r="B25" t="n">
-        <v>0.002781870814260946</v>
+        <v>0.002770960498583504</v>
       </c>
       <c r="C25" t="n">
-        <v>0.003821456776436243</v>
+        <v>0.00382153294162884</v>
       </c>
     </row>
     <row r="26">
@@ -769,10 +769,10 @@
         </is>
       </c>
       <c r="B26" t="n">
-        <v>0.00252220947213345</v>
+        <v>0.002513968040776969</v>
       </c>
       <c r="C26" t="n">
-        <v>0.01424756738977666</v>
+        <v>0.01424787278658742</v>
       </c>
     </row>
     <row r="27">
@@ -782,10 +782,10 @@
         </is>
       </c>
       <c r="B27" t="n">
-        <v>0.002147623476053842</v>
+        <v>0.002161830910220478</v>
       </c>
       <c r="C27" t="n">
-        <v>0.005794436636669871</v>
+        <v>0.005792981022725371</v>
       </c>
     </row>
     <row r="28">
@@ -795,10 +795,10 @@
         </is>
       </c>
       <c r="B28" t="n">
-        <v>0.001873392613959506</v>
+        <v>0.001871461435310012</v>
       </c>
       <c r="C28" t="n">
-        <v>0.004413456573095305</v>
+        <v>0.0044129449254809</v>
       </c>
     </row>
     <row r="29">
@@ -808,10 +808,10 @@
         </is>
       </c>
       <c r="B29" t="n">
-        <v>0.001699203972424952</v>
+        <v>0.001682369574197435</v>
       </c>
       <c r="C29" t="n">
-        <v>0.008777499981835505</v>
+        <v>0.008779061339318913</v>
       </c>
     </row>
     <row r="30">
@@ -821,10 +821,10 @@
         </is>
       </c>
       <c r="B30" t="n">
-        <v>0.001114679125439957</v>
+        <v>0.001127481676276427</v>
       </c>
       <c r="C30" t="n">
-        <v>0.003679986208948686</v>
+        <v>0.003674850260214023</v>
       </c>
     </row>
     <row r="31">
@@ -834,10 +834,10 @@
         </is>
       </c>
       <c r="B31" t="n">
-        <v>0.001114539004016582</v>
+        <v>0.001114087098221209</v>
       </c>
       <c r="C31" t="n">
-        <v>0.005383322959193828</v>
+        <v>0.00538171850729139</v>
       </c>
     </row>
   </sheetData>

</xml_diff>